<commit_message>
show connections valgrind arreglat
</commit_message>
<xml_diff>
--- a/HoresPracticaSO.xlsx
+++ b/HoresPracticaSO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aridaniele/Library/Mobile Documents/com~apple~CloudDocs/UNI/3/SO/PracticaSO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aridaniele/Documents/Documentos_MacBookProdeAri/UNI/3/SO/PracticaSO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3094C251-CAA6-734B-988E-4459357D0E47}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E52EA1-F43B-F04E-AB6C-3C95B31C5C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{FAA491D1-5501-3E4C-A385-6E71341EFC52}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{FAA491D1-5501-3E4C-A385-6E71341EFC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Hores</t>
   </si>
   <si>
-    <t>Tasca</t>
-  </si>
-  <si>
     <t>Plantejament</t>
   </si>
   <si>
@@ -52,6 +49,24 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>Fase 1</t>
+  </si>
+  <si>
+    <t>Fase 2</t>
+  </si>
+  <si>
+    <t>Opció Connect</t>
+  </si>
+  <si>
+    <t>Opció Show Connections</t>
+  </si>
+  <si>
+    <t>Opció Say</t>
+  </si>
+  <si>
+    <t>Opció Exit</t>
   </si>
 </sst>
 </file>
@@ -403,17 +418,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55943EE-4122-4945-93C5-9A66BA157BE2}">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -421,15 +436,15 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -437,7 +452,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -445,7 +460,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -453,18 +468,55 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hores update aunque ya suda
</commit_message>
<xml_diff>
--- a/HoresPracticaSO.xlsx
+++ b/HoresPracticaSO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clara\Documents\_UNI\3r\SO\Pràctica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aridaniele/Documents/Documentos_MacBookProdeAri/UNI/3/SO/PracticaSO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD454CC-9559-4C98-B8AF-E1838BCC9962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5ED903-A0CF-8C45-9376-869B0118CAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FAA491D1-5501-3E4C-A385-6E71341EFC52}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16300" xr2:uid="{FAA491D1-5501-3E4C-A385-6E71341EFC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Hores</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Valgrind</t>
+  </si>
+  <si>
+    <t>Fase 4</t>
+  </si>
+  <si>
+    <t>Broadcast</t>
+  </si>
+  <si>
+    <t>Memòria</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55943EE-4122-4945-93C5-9A66BA157BE2}">
-  <dimension ref="B2:C24"/>
+  <dimension ref="B2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -449,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -457,7 +466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -465,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -473,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -481,7 +490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -489,7 +498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -497,12 +506,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -510,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -518,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -526,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -534,12 +543,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>15</v>
       </c>
@@ -547,7 +556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -555,7 +564,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -563,12 +572,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24">
         <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>